<commit_message>
Load 14: Pivote Table
</commit_message>
<xml_diff>
--- a/data/raw/Fitchi/SHSZ300 Index.xlsx
+++ b/data/raw/Fitchi/SHSZ300 Index.xlsx
@@ -1,20 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\k.vinogradov\Documents\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Forex-and-Stock-Python-Trade-Model\data\raw\Fitchi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A6D2D1-B2D4-4064-85D3-D07D48CF0979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="-105" windowWidth="14850" windowHeight="12735"/>
+    <workbookView xWindow="-109" yWindow="-14780" windowWidth="26301" windowHeight="14427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -63,10 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="182" formatCode="dd\.mm\.yyyy"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,56 +559,55 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="blp_datetime" xfId="42"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="blp_datetime" xfId="42" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Акцент1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Заголовок 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заголовок 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заголовок 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Заголовок 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="29" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -615,41 +622,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="bloomberg.rtd">
-      <tp>
-        <v>43634</v>
-        <stp/>
-        <stp>##V3_BDHV12</stp>
-        <stp xml:space="preserve">SHSZ300 Index                                                   </stp>
-        <stp>PX_LAST_x0002_PX_HIGH</stp>
-        <stp>04.01.2005</stp>
-        <stp>18.06.2019</stp>
-        <stp>[grid1_ikcitt43.xlsx]Worksheet!R8C1</stp>
-        <stp>Dir=V</stp>
-        <stp>Dts=S</stp>
-        <stp>Sort=D</stp>
-        <stp>Quote=C</stp>
-        <stp>QtTyp=P</stp>
-        <stp>Days=T</stp>
-        <stp>Per=cD</stp>
-        <stp>DtFmt=D</stp>
-        <stp>UseDPDF=Y</stp>
-        <stp>FX=CNY</stp>
-        <stp>cols=3;rows=3512</stp>
-        <tr r="A8" s="2"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -687,7 +663,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -722,6 +698,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -757,9 +750,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -932,20 +942,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3519"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +973,10 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>38356</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>38356</v>
       </c>
     </row>
@@ -974,10 +984,10 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>43634</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>43634</v>
       </c>
     </row>
@@ -1021,8 +1031,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <f>_xll.BDH(B1,B7:C7,B2,B3,"Dir=V","Dts=S","Sort=D","Quote=C","QtTyp=P","Days=T",CONCATENATE("Per=c",B4),"DtFmt=D","UseDPDF=Y",CONCATENATE("FX=",B5),"cols=3;rows=3512")</f>
+      <c r="A8" s="1">
         <v>43634</v>
       </c>
       <c r="B8">

</xml_diff>